<commit_message>
Implement get_contact() to fetch representative info from entities listed in an Excel file. Add new Excel file with entity contact info.
</commit_message>
<xml_diff>
--- a/Excel2Xml/representantes_de_entidades.xlsx
+++ b/Excel2Xml/representantes_de_entidades.xlsx
@@ -13,7 +13,7 @@
     <sheet name="Entidades" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Entidades!$B$2:$B$40</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Entidades!$B$2:$B$39</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="286">
   <si>
     <t xml:space="preserve">EXPORTADORA TAVAREZ ET. S.R.L.</t>
   </si>
@@ -883,21 +883,6 @@
   </si>
   <si>
     <t xml:space="preserve">JUAN SANCHEZ RAMIREZ, No. 42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGROCOMERCIAL MANUEL GARCIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CEDULA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">071-0027380-9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">809     - 584-2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES NAGUA</t>
   </si>
 </sst>
 </file>
@@ -1036,7 +1021,7 @@
       <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="78.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.86"/>
@@ -1219,7 +1204,7 @@
       <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="86.12"/>
   </cols>
@@ -1317,13 +1302,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="93.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.57"/>
@@ -2731,46 +2716,8 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>286</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>273</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>287</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>288</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="F37" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="G37" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="H37" s="4" t="n">
-        <v>23710</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="J37" s="0" t="s">
-        <v>289</v>
-      </c>
-      <c r="K37" s="0" t="s">
-        <v>290</v>
-      </c>
-      <c r="L37" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="B2:B40"/>
+  <autoFilter ref="B2:B39"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Create simple_converter_2.py, implement Factory DP to simple_converter.py. Update representantes_de_entidades.xlsx. Add May and July excel files.
</commit_message>
<xml_diff>
--- a/Excel2Xml/representantes_de_entidades.xlsx
+++ b/Excel2Xml/representantes_de_entidades.xlsx
@@ -13,7 +13,7 @@
     <sheet name="Entidades" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Entidades!$B$2:$B$39</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Entidades!$B$2:$B$36</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="310">
   <si>
     <t xml:space="preserve">EXPORTADORA TAVAREZ ET. S.R.L.</t>
   </si>
@@ -156,7 +156,7 @@
     <t xml:space="preserve">1-02-34223-7        </t>
   </si>
   <si>
-    <t xml:space="preserve">ENTIDAD</t>
+    <t xml:space="preserve">CLIENTE</t>
   </si>
   <si>
     <t xml:space="preserve">NOMBRE COMERCIAL</t>
@@ -285,13 +285,22 @@
     <t xml:space="preserve">LOS PINOS OESTE, RECIDENCIAL CARMEN MARIA</t>
   </si>
   <si>
-    <t xml:space="preserve">TEMPORALMENTE NO DISPONIBLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">000-0000000-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">809     - 222-2222  </t>
+    <t xml:space="preserve">FRANCISCO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GARCIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">001-0586646-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">809     - 258-2085  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLAZA LA BANDERA, 27 DE FEBRERO, SANTO DOMINGO, D.N.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGRONOMO</t>
   </si>
   <si>
     <t xml:space="preserve">PABLO</t>
@@ -399,9 +408,6 @@
     <t xml:space="preserve">APABY</t>
   </si>
   <si>
-    <t xml:space="preserve">FRANCISCO</t>
-  </si>
-  <si>
     <t xml:space="preserve">FRIAS</t>
   </si>
   <si>
@@ -600,9 +606,6 @@
     <t xml:space="preserve">RADHAMES</t>
   </si>
   <si>
-    <t xml:space="preserve">GARCIA</t>
-  </si>
-  <si>
     <t xml:space="preserve">054-0066632-6      </t>
   </si>
   <si>
@@ -705,9 +708,6 @@
     <t xml:space="preserve">C/RAFAEL AUGUSTO SANCHEZ, EVARISTO MORALES, SANTO DOMINGO</t>
   </si>
   <si>
-    <t xml:space="preserve">AGRONOMO</t>
-  </si>
-  <si>
     <t xml:space="preserve">PROC. GEN</t>
   </si>
   <si>
@@ -883,6 +883,78 @@
   </si>
   <si>
     <t xml:space="preserve">JUAN SANCHEZ RAMIREZ, No. 42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXPORTADORA TAVAREZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E.T                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAVAREZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15/07/1949</t>
+  </si>
+  <si>
+    <t xml:space="preserve">048-0036928-4       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">809    - 757-0471  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES LAS MANDARINAS, No. 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMERCIANTES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOSE EMILIO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SANTIAGO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CEDULA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">055-0002602-5       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROSA MARIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FERREIRAS           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">055-0000156-4       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">809    - 577-2629  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SALCEDO                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NIKAY BIO-PROC      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-30-23609-7        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CESAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AYBAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">001-007162-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">809-537-3106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C/ BENITO MONCION, No. 10, apt. 4</t>
   </si>
 </sst>
 </file>
@@ -893,7 +965,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$-409]m/d/yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -919,6 +991,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF111111"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -965,7 +1044,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -982,6 +1061,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -990,8 +1073,8 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1003,6 +1086,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF111111"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -1021,7 +1164,7 @@
       <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="78.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.86"/>
@@ -1204,7 +1347,7 @@
       <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="86.12"/>
   </cols>
@@ -1302,13 +1445,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:M98"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M39" activeCellId="0" sqref="M39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="93.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.57"/>
@@ -1339,31 +1482,31 @@
       <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="3" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1389,10 +1532,10 @@
       <c r="G2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H2" s="4" t="n">
+      <c r="H2" s="5" t="n">
         <v>11086</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="6" t="s">
         <v>61</v>
       </c>
       <c r="J2" s="1" t="s">
@@ -1430,10 +1573,10 @@
       <c r="G3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H3" s="4" t="n">
+      <c r="H3" s="5" t="n">
         <v>24079</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="6" t="s">
         <v>69</v>
       </c>
       <c r="J3" s="1" t="s">
@@ -1471,10 +1614,10 @@
       <c r="G4" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H4" s="4" t="n">
+      <c r="H4" s="5" t="n">
         <v>27750</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="6" t="s">
         <v>78</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -1509,10 +1652,10 @@
       <c r="G5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="4" t="n">
+      <c r="H5" s="5" t="n">
         <v>27087</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="6" t="s">
         <v>83</v>
       </c>
       <c r="J5" s="1" t="s">
@@ -1543,25 +1686,28 @@
         <v>86</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G6" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="H6" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="J6" s="0" t="s">
+      <c r="H6" s="5" t="n">
+        <v>19635</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>88</v>
       </c>
+      <c r="J6" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="K6" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="L6" s="0" t="s">
         <v>64</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1578,25 +1724,25 @@
         <v>14</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="G7" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="H7" s="4" t="n">
+      <c r="H7" s="5" t="n">
         <v>21164</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>92</v>
+      <c r="I7" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>64</v>
@@ -1607,7 +1753,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>1</v>
@@ -1616,25 +1762,25 @@
         <v>22</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="H8" s="4" t="n">
+      <c r="H8" s="5" t="n">
         <v>20199</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>98</v>
+      <c r="I8" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>64</v>
@@ -1642,37 +1788,37 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="H9" s="4" t="n">
+      <c r="H9" s="5" t="n">
         <v>15910</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>106</v>
+      <c r="I9" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="L9" s="0" t="s">
         <v>64</v>
@@ -1683,7 +1829,7 @@
         <v>29</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>1</v>
@@ -1692,25 +1838,25 @@
         <v>30</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="H10" s="4" t="n">
+      <c r="H10" s="5" t="n">
         <v>23012</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="J10" s="0" t="s">
-        <v>112</v>
+      <c r="I10" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="L10" s="0" t="s">
         <v>64</v>
@@ -1718,37 +1864,37 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="H11" s="4" t="n">
+      <c r="H11" s="5" t="n">
         <v>22110</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>120</v>
+      <c r="I11" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="L11" s="0" t="s">
         <v>64</v>
@@ -1759,7 +1905,7 @@
         <v>27</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>1</v>
@@ -1768,25 +1914,25 @@
         <v>28</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="H12" s="4" t="n">
+      <c r="H12" s="5" t="n">
         <v>15910</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="J12" s="0" t="s">
-        <v>106</v>
+      <c r="I12" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="L12" s="0" t="s">
         <v>64</v>
@@ -1797,7 +1943,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>1</v>
@@ -1806,25 +1952,25 @@
         <v>26</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>124</v>
+        <v>86</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G13" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="H13" s="4" t="n">
+      <c r="H13" s="5" t="n">
         <v>22556</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="J13" s="0" t="s">
-        <v>127</v>
+      <c r="I13" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="L13" s="0" t="s">
         <v>64</v>
@@ -1832,19 +1978,19 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>82</v>
@@ -1852,17 +1998,17 @@
       <c r="G14" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="H14" s="4" t="n">
+      <c r="H14" s="5" t="n">
         <v>18835</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="J14" s="0" t="s">
-        <v>134</v>
+      <c r="I14" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L14" s="0" t="s">
         <v>64</v>
@@ -1870,37 +2016,37 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G15" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="H15" s="4" t="n">
+      <c r="H15" s="5" t="n">
         <v>24836</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="J15" s="0" t="s">
-        <v>142</v>
+      <c r="I15" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="L15" s="0" t="s">
         <v>64</v>
@@ -1908,37 +2054,37 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="G16" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="H16" s="4" t="n">
+      <c r="H16" s="5" t="n">
         <v>22762</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="J16" s="0" t="s">
-        <v>150</v>
+      <c r="I16" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="L16" s="0" t="s">
         <v>64</v>
@@ -1946,37 +2092,37 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H17" s="4" t="n">
+      <c r="H17" s="5" t="n">
         <v>26447</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>158</v>
+      <c r="I17" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>160</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="L17" s="0" t="s">
         <v>64</v>
@@ -1984,10 +2130,10 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>1</v>
@@ -1996,25 +2142,25 @@
         <v>16</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H18" s="4" t="n">
+      <c r="H18" s="5" t="n">
         <v>22175</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>165</v>
+      <c r="I18" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>167</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="L18" s="0" t="s">
         <v>64</v>
@@ -2025,7 +2171,7 @@
         <v>3</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>1</v>
@@ -2034,25 +2180,25 @@
         <v>4</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H19" s="4" t="n">
+      <c r="H19" s="5" t="n">
         <v>23881</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>171</v>
+      <c r="I19" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>173</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="L19" s="0" t="s">
         <v>64</v>
@@ -2060,37 +2206,37 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H20" s="4" t="n">
+      <c r="H20" s="5" t="n">
         <v>23026</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="L20" s="0" t="s">
         <v>64</v>
@@ -2101,7 +2247,7 @@
         <v>23</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>1</v>
@@ -2110,25 +2256,25 @@
         <v>24</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="4" t="n">
+      <c r="H21" s="5" t="n">
         <v>16044</v>
       </c>
-      <c r="I21" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>185</v>
+      <c r="I21" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>187</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="L21" s="0" t="s">
         <v>64</v>
@@ -2136,37 +2282,37 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>191</v>
+        <v>87</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H22" s="4" t="n">
+      <c r="H22" s="5" t="n">
         <v>27795</v>
       </c>
-      <c r="I22" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="J22" s="3" t="s">
+      <c r="I22" s="6" t="s">
         <v>193</v>
       </c>
+      <c r="J22" s="1" t="s">
+        <v>194</v>
+      </c>
       <c r="K22" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="L22" s="0" t="s">
         <v>64</v>
@@ -2174,10 +2320,10 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>1</v>
@@ -2186,25 +2332,25 @@
         <v>32</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H23" s="4" t="n">
+      <c r="H23" s="5" t="n">
         <v>16354</v>
       </c>
-      <c r="I23" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="J23" s="3" t="s">
+      <c r="I23" s="6" t="s">
         <v>200</v>
       </c>
+      <c r="J23" s="1" t="s">
+        <v>201</v>
+      </c>
       <c r="K23" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="L23" s="0" t="s">
         <v>64</v>
@@ -2212,37 +2358,37 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H24" s="4" t="n">
+      <c r="H24" s="5" t="n">
         <v>24024</v>
       </c>
-      <c r="I24" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="J24" s="3" t="s">
+      <c r="I24" s="6" t="s">
         <v>208</v>
       </c>
+      <c r="J24" s="1" t="s">
+        <v>209</v>
+      </c>
       <c r="K24" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="L24" s="0" t="s">
         <v>64</v>
@@ -2253,7 +2399,7 @@
         <v>11</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>1</v>
@@ -2262,25 +2408,25 @@
         <v>12</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H25" s="4" t="n">
+      <c r="H25" s="5" t="n">
         <v>24754</v>
       </c>
-      <c r="I25" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="J25" s="3" t="s">
+      <c r="I25" s="6" t="s">
         <v>213</v>
       </c>
+      <c r="J25" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="K25" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="L25" s="0" t="s">
         <v>64</v>
@@ -2291,7 +2437,7 @@
         <v>19</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>1</v>
@@ -2300,25 +2446,25 @@
         <v>20</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H26" s="4" t="n">
+      <c r="H26" s="5" t="n">
         <v>19956</v>
       </c>
-      <c r="I26" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="J26" s="3" t="s">
+      <c r="I26" s="6" t="s">
         <v>219</v>
       </c>
+      <c r="J26" s="1" t="s">
+        <v>220</v>
+      </c>
       <c r="K26" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="L26" s="0" t="s">
         <v>64</v>
@@ -2329,7 +2475,7 @@
         <v>7</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>1</v>
@@ -2338,31 +2484,31 @@
         <v>8</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H27" s="4" t="n">
+      <c r="H27" s="5" t="n">
         <v>18089</v>
       </c>
-      <c r="I27" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="J27" s="3" t="s">
+      <c r="I27" s="6" t="s">
         <v>224</v>
       </c>
+      <c r="J27" s="1" t="s">
+        <v>225</v>
+      </c>
       <c r="K27" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="L27" s="0" t="s">
         <v>64</v>
       </c>
       <c r="M27" s="0" t="s">
-        <v>226</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2387,13 +2533,13 @@
       <c r="G28" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H28" s="4" t="n">
+      <c r="H28" s="5" t="n">
         <v>19665</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="I28" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="J28" s="0" t="s">
+      <c r="J28" s="1" t="s">
         <v>231</v>
       </c>
       <c r="K28" s="0" t="s">
@@ -2425,13 +2571,13 @@
       <c r="G29" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H29" s="4" t="n">
+      <c r="H29" s="5" t="n">
         <v>24289</v>
       </c>
-      <c r="I29" s="2" t="s">
+      <c r="I29" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="J29" s="0" t="s">
+      <c r="J29" s="1" t="s">
         <v>239</v>
       </c>
       <c r="K29" s="0" t="s">
@@ -2463,13 +2609,13 @@
       <c r="G30" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H30" s="4" t="n">
+      <c r="H30" s="5" t="n">
         <v>25034</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="I30" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="J30" s="0" t="s">
+      <c r="J30" s="1" t="s">
         <v>245</v>
       </c>
       <c r="K30" s="0" t="s">
@@ -2501,13 +2647,13 @@
       <c r="G31" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="H31" s="4" t="n">
+      <c r="H31" s="5" t="n">
         <v>26315</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="I31" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="J31" s="0" t="s">
+      <c r="J31" s="1" t="s">
         <v>250</v>
       </c>
       <c r="K31" s="0" t="s">
@@ -2542,13 +2688,13 @@
       <c r="G32" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H32" s="4" t="n">
+      <c r="H32" s="5" t="n">
         <v>31777</v>
       </c>
-      <c r="I32" s="2" t="s">
+      <c r="I32" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="J32" s="0" t="s">
+      <c r="J32" s="1" t="s">
         <v>256</v>
       </c>
       <c r="K32" s="0" t="s">
@@ -2575,18 +2721,18 @@
         <v>261</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H33" s="4" t="n">
+      <c r="H33" s="5" t="n">
         <v>20718</v>
       </c>
-      <c r="I33" s="2" t="s">
+      <c r="I33" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="J33" s="0" t="s">
+      <c r="J33" s="1" t="s">
         <v>263</v>
       </c>
       <c r="K33" s="0" t="s">
@@ -2621,13 +2767,13 @@
       <c r="G34" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H34" s="4" t="n">
+      <c r="H34" s="5" t="n">
         <v>32606</v>
       </c>
-      <c r="I34" s="2" t="s">
+      <c r="I34" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="J34" s="0" t="s">
+      <c r="J34" s="1" t="s">
         <v>271</v>
       </c>
       <c r="K34" s="0" t="s">
@@ -2659,13 +2805,13 @@
       <c r="G35" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="H35" s="4" t="n">
+      <c r="H35" s="5" t="n">
         <v>23603</v>
       </c>
-      <c r="I35" s="2" t="s">
+      <c r="I35" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="J35" s="0" t="s">
+      <c r="J35" s="1" t="s">
         <v>277</v>
       </c>
       <c r="K35" s="0" t="s">
@@ -2697,13 +2843,13 @@
       <c r="G36" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H36" s="4" t="n">
+      <c r="H36" s="5" t="n">
         <v>17652</v>
       </c>
-      <c r="I36" s="2" t="s">
+      <c r="I36" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="J36" s="0" t="s">
+      <c r="J36" s="1" t="s">
         <v>284</v>
       </c>
       <c r="K36" s="0" t="s">
@@ -2716,8 +2862,388 @@
         <v>65</v>
       </c>
     </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="K37" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="L37" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="M37" s="0" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="H38" s="5" t="n">
+        <v>20529</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="H39" s="5" t="n">
+        <v>-342548</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="K39" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="L39" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H40" s="5"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H41" s="5"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H42" s="5"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H43" s="5"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H44" s="5"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H45" s="5"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H46" s="5"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="1"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H47" s="5"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H48" s="5"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="1"/>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H49" s="5"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="1"/>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H50" s="5"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="1"/>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H51" s="5"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H52" s="5"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="1"/>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H53" s="5"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="1"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H54" s="5"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="1"/>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H55" s="5"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="1"/>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H56" s="5"/>
+      <c r="I56" s="6"/>
+      <c r="J56" s="1"/>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H57" s="5"/>
+      <c r="I57" s="6"/>
+      <c r="J57" s="1"/>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H58" s="5"/>
+      <c r="I58" s="6"/>
+      <c r="J58" s="1"/>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H59" s="5"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="1"/>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H60" s="5"/>
+      <c r="I60" s="6"/>
+      <c r="J60" s="1"/>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H61" s="5"/>
+      <c r="I61" s="6"/>
+      <c r="J61" s="1"/>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H62" s="5"/>
+      <c r="I62" s="6"/>
+      <c r="J62" s="1"/>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H63" s="5"/>
+      <c r="I63" s="6"/>
+      <c r="J63" s="1"/>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H64" s="5"/>
+      <c r="I64" s="6"/>
+      <c r="J64" s="1"/>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H65" s="5"/>
+      <c r="I65" s="6"/>
+      <c r="J65" s="1"/>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H66" s="5"/>
+      <c r="I66" s="6"/>
+      <c r="J66" s="1"/>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H67" s="5"/>
+      <c r="I67" s="6"/>
+      <c r="J67" s="1"/>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H68" s="5"/>
+      <c r="I68" s="6"/>
+      <c r="J68" s="1"/>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H69" s="5"/>
+      <c r="I69" s="6"/>
+      <c r="J69" s="1"/>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H70" s="5"/>
+      <c r="I70" s="6"/>
+      <c r="J70" s="1"/>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H71" s="5"/>
+      <c r="I71" s="6"/>
+      <c r="J71" s="1"/>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H72" s="5"/>
+      <c r="I72" s="6"/>
+      <c r="J72" s="1"/>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H73" s="5"/>
+      <c r="I73" s="6"/>
+      <c r="J73" s="1"/>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H74" s="5"/>
+      <c r="I74" s="6"/>
+      <c r="J74" s="1"/>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H75" s="5"/>
+      <c r="I75" s="6"/>
+      <c r="J75" s="1"/>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H76" s="5"/>
+      <c r="I76" s="6"/>
+      <c r="J76" s="1"/>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H77" s="5"/>
+      <c r="I77" s="6"/>
+      <c r="J77" s="1"/>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H78" s="5"/>
+      <c r="I78" s="6"/>
+      <c r="J78" s="1"/>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H79" s="5"/>
+      <c r="I79" s="6"/>
+      <c r="J79" s="1"/>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H80" s="5"/>
+      <c r="I80" s="6"/>
+      <c r="J80" s="1"/>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H81" s="5"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="1"/>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H82" s="5"/>
+      <c r="I82" s="6"/>
+      <c r="J82" s="1"/>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H83" s="5"/>
+      <c r="I83" s="6"/>
+      <c r="J83" s="1"/>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J84" s="1"/>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J85" s="1"/>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J86" s="1"/>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J87" s="1"/>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J88" s="1"/>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J89" s="1"/>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J90" s="1"/>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J91" s="1"/>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J92" s="1"/>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J93" s="1"/>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J94" s="1"/>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J95" s="1"/>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J96" s="1"/>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J97" s="1"/>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J98" s="1"/>
+    </row>
   </sheetData>
-  <autoFilter ref="B2:B39"/>
+  <autoFilter ref="B2:B36"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>